<commit_message>
Updated the validation matrices for the showcase scenarios to use our markdown format rather than pdfs, updated the references in sources.bib, and updated the System Methodology report with the new matrices and outlined new required tables. Still finishing the showcase scenarios.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\Showcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C82BC0D-5DD7-4A21-873A-4F8A27453F62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4071023F-EEED-40BA-9015-4CC1D3E3E258}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="255" windowWidth="20565" windowHeight="14700" tabRatio="329" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="24825" windowHeight="11385" tabRatio="406" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthma Attack Overview" sheetId="8" r:id="rId1"/>
-    <sheet name="Asthma Attack Breakdown" sheetId="9" r:id="rId2"/>
+    <sheet name="Asthma Attack Breakdown" sheetId="9" state="hidden" r:id="rId2"/>
+    <sheet name="Asthma Attack" sheetId="10" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Asthma Attack Breakdown'!$A$1:$BM$8</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="211">
   <si>
     <t>Scenario Overview</t>
   </si>
@@ -725,6 +726,164 @@
   </si>
   <si>
     <t>Back to baseline [2],[5]</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Action Occurrence Time  (s)</t>
+  </si>
+  <si>
+    <t>Sample Scenario Time  (s)</t>
+  </si>
+  <si>
+    <t>Heart Rate  (beats/min)</t>
+  </si>
+  <si>
+    <t>Systolic Pressure  (mmHg)</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>|&lt;span class="success"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/span&gt;|&lt;span class="success"&gt;</t>
+  </si>
+  <si>
+    <t>Begin Asthma Attack
+(Severity 0.7)</t>
+  </si>
+  <si>
+    <t>Administer Albuterol
+(Albuterol inhaler used correctly, 90.0 ug dose, nozzle loss fraction 0.04)</t>
+  </si>
+  <si>
+    <t>10 minutes of asthma attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug Onset in &lt; </t>
+  </si>
+  <si>
+    <t>Heart Stroke Volume (mL)</t>
+  </si>
+  <si>
+    <t>Mean Arterial Pressure  (mmHg)</t>
+  </si>
+  <si>
+    <t>Cardiac Output (mL/min)</t>
+  </si>
+  <si>
+    <t>Respiration Rate (breaths/min)</t>
+  </si>
+  <si>
+    <t>Oxygen Saturation (fraction)</t>
+  </si>
+  <si>
+    <t>End Tidal CO2 (fraction)</t>
+  </si>
+  <si>
+    <t>PaO2 (mmHg)</t>
+  </si>
+  <si>
+    <t>PaCO2 (mmHg)</t>
+  </si>
+  <si>
+    <t>pH (mmHg)</t>
+  </si>
+  <si>
+    <t>Increase @cite adams2012patient</t>
+  </si>
+  <si>
+    <t>Decrease @cite adams2012patient</t>
+  </si>
+  <si>
+    <t>&lt;/span&gt;|&lt;span class="danger"&gt;</t>
+  </si>
+  <si>
+    <t>|&lt;span class="danger"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/span&gt;|&lt;span class="warning"&gt;</t>
+  </si>
+  <si>
+    <t>Decrease @cite bergeronSME
+Decrease is expected with increased heart rate</t>
+  </si>
+  <si>
+    <t>No Change @cite bergeronSME</t>
+  </si>
+  <si>
+    <t>Increase  @cite adams2012patient</t>
+  </si>
+  <si>
+    <t>Decrease  @cite adams2012patient</t>
+  </si>
+  <si>
+    <t>Increase back to baseline  @cite adams2012patient</t>
+  </si>
+  <si>
+    <t>Increase  @cite adams2012patient @cite Raimondi2013acid</t>
+  </si>
+  <si>
+    <t>Decrease  @cite adams2012patient @cite Raimondi2013acid</t>
+  </si>
+  <si>
+    <t>Decreased peak @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <t>71.5 ± 12 @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <t>78.0 ± 12.7 @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <t>32.3 ± 4.6 @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <t>35.8 ± 6.9 @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <r>
+      <t>Back to baseline @cite Mountain1990acid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> @cite </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Raimondi2013acid</t>
+    </r>
+  </si>
+  <si>
+    <t>Increase @cite Mountain1990acid @cite Raimondi2013acid</t>
+  </si>
+  <si>
+    <t>Back to baseline @cite metoyer2016SME</t>
+  </si>
+  <si>
+    <t>&lt;/span&gt;|</t>
   </si>
 </sst>
 </file>
@@ -948,7 +1107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1060,6 +1219,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1067,7 +1252,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1331,6 +1516,30 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1372,6 +1581,15 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1719,8 +1937,8 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:D12"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,20 +1949,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="105"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="113"/>
     </row>
     <row r="2" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="114" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="102"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="110"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1775,52 +1993,52 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="108"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="116"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="102"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="110"/>
     </row>
     <row r="7" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="102"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="110"/>
     </row>
     <row r="8" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="110"/>
     </row>
     <row r="9" spans="1:4" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="101"/>
-      <c r="D9" s="102"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="110"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
@@ -1840,61 +2058,61 @@
       <c r="A12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="105" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="98"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="106"/>
     </row>
     <row r="13" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="110"/>
     </row>
     <row r="14" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="110"/>
     </row>
     <row r="15" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="101"/>
-      <c r="D15" s="102"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="110"/>
     </row>
     <row r="16" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="101" t="s">
+      <c r="B16" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="102"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="110"/>
     </row>
     <row r="17" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="109" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="101"/>
-      <c r="D17" s="102"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="110"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
@@ -1908,21 +2126,21 @@
       <c r="A19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="97" t="s">
+      <c r="B19" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="98"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="99"/>
-      <c r="D20" s="100"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="108"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
@@ -2000,11 +2218,11 @@
   </sheetPr>
   <dimension ref="A1:BM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" ySplit="23" topLeftCell="BH24" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" ySplit="23" topLeftCell="AL24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="BK11" sqref="BK11"/>
+      <selection pane="bottomRight" activeCell="AT5" sqref="AT5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2872,34 +3090,34 @@
       <c r="BM6" s="90"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="109"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
     </row>
     <row r="8" spans="1:65" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="60"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
-      <c r="G8" s="110" t="s">
+      <c r="G8" s="118" t="s">
         <v>161</v>
       </c>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="110"/>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="110"/>
-      <c r="S8" s="110"/>
-      <c r="T8" s="110"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="118"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="118"/>
+      <c r="Q8" s="118"/>
+      <c r="R8" s="118"/>
+      <c r="S8" s="118"/>
+      <c r="T8" s="118"/>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="C9" s="62"/>
@@ -2935,4 +3153,442 @@
     <oddHeader>&amp;A</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820C7F09-B001-4E49-B466-E1E2EF602302}">
+  <dimension ref="A1:AE7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AE1" sqref="A1:AE4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" customWidth="1"/>
+    <col min="27" max="27" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" customWidth="1"/>
+    <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="98" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="98" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="99" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="99" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="L1" s="100" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" s="100" t="s">
+        <v>182</v>
+      </c>
+      <c r="O1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="R1" s="100" t="s">
+        <v>183</v>
+      </c>
+      <c r="S1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="T1" s="100" t="s">
+        <v>184</v>
+      </c>
+      <c r="U1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="V1" s="100" t="s">
+        <v>185</v>
+      </c>
+      <c r="W1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="X1" s="100" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z1" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" s="100" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC1" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD1" s="100" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE1" s="97" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="I2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="J2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="M2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="O2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="R2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="S2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="T2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="U2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="V2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="W2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="X2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="AC2" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD2" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE2" s="97" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="101">
+        <v>60</v>
+      </c>
+      <c r="G3" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="101">
+        <v>660</v>
+      </c>
+      <c r="I3" s="97" t="s">
+        <v>175</v>
+      </c>
+      <c r="J3" s="104" t="s">
+        <v>190</v>
+      </c>
+      <c r="K3" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" s="104" t="s">
+        <v>195</v>
+      </c>
+      <c r="M3" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="N3" s="104" t="s">
+        <v>190</v>
+      </c>
+      <c r="O3" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="P3" s="103" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q3" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="R3" s="103" t="s">
+        <v>197</v>
+      </c>
+      <c r="S3" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="T3" s="104" t="s">
+        <v>200</v>
+      </c>
+      <c r="U3" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="V3" s="104" t="s">
+        <v>198</v>
+      </c>
+      <c r="W3" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="X3" s="104" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y3" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z3" s="104" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA3" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB3" s="104" t="s">
+        <v>206</v>
+      </c>
+      <c r="AC3" s="97" t="s">
+        <v>192</v>
+      </c>
+      <c r="AD3" s="102" t="s">
+        <v>208</v>
+      </c>
+      <c r="AE3" s="97" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="78" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="101">
+        <v>660</v>
+      </c>
+      <c r="G4" s="97" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="101">
+        <v>960</v>
+      </c>
+      <c r="I4" s="97" t="s">
+        <v>193</v>
+      </c>
+      <c r="J4" s="102" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="L4" s="103" t="s">
+        <v>196</v>
+      </c>
+      <c r="M4" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="N4" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="O4" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="P4" s="104" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q4" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="R4" s="103" t="s">
+        <v>196</v>
+      </c>
+      <c r="S4" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="T4" s="104" t="s">
+        <v>201</v>
+      </c>
+      <c r="U4" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="V4" s="104" t="s">
+        <v>199</v>
+      </c>
+      <c r="W4" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="X4" s="103" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y4" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z4" s="104" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA4" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB4" s="104" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC4" s="97" t="s">
+        <v>176</v>
+      </c>
+      <c r="AD4" s="104" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE4" s="120" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD5" s="119"/>
+      <c r="AE5" s="121"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE6" s="121"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE7" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes to showcase matrices and adding a reference to the source.bib.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\Showcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4071023F-EEED-40BA-9015-4CC1D3E3E258}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E80D08-D6F6-420A-BB7D-C5A8E2AD1815}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="24825" windowHeight="11385" tabRatio="406" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="24825" windowHeight="11385" tabRatio="406" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asthma Attack Overview" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="210">
   <si>
     <t>Scenario Overview</t>
   </si>
@@ -758,20 +758,9 @@
     <t>&lt;/span&gt;|&lt;span class="success"&gt;</t>
   </si>
   <si>
-    <t>Begin Asthma Attack
-(Severity 0.7)</t>
-  </si>
-  <si>
-    <t>Administer Albuterol
-(Albuterol inhaler used correctly, 90.0 ug dose, nozzle loss fraction 0.04)</t>
-  </si>
-  <si>
     <t>10 minutes of asthma attack</t>
   </si>
   <si>
-    <t xml:space="preserve">Drug Onset in &lt; </t>
-  </si>
-  <si>
     <t>Heart Stroke Volume (mL)</t>
   </si>
   <si>
@@ -814,28 +803,12 @@
     <t>&lt;/span&gt;|&lt;span class="warning"&gt;</t>
   </si>
   <si>
-    <t>Decrease @cite bergeronSME
-Decrease is expected with increased heart rate</t>
-  </si>
-  <si>
     <t>No Change @cite bergeronSME</t>
   </si>
   <si>
     <t>Increase  @cite adams2012patient</t>
   </si>
   <si>
-    <t>Decrease  @cite adams2012patient</t>
-  </si>
-  <si>
-    <t>Increase back to baseline  @cite adams2012patient</t>
-  </si>
-  <si>
-    <t>Increase  @cite adams2012patient @cite Raimondi2013acid</t>
-  </si>
-  <si>
-    <t>Decrease  @cite adams2012patient @cite Raimondi2013acid</t>
-  </si>
-  <si>
     <t>Decreased peak @cite Nowak1983arterial</t>
   </si>
   <si>
@@ -851,32 +824,6 @@
     <t>35.8 ± 6.9 @cite Nowak1983arterial</t>
   </si>
   <si>
-    <r>
-      <t>Back to baseline @cite Mountain1990acid</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> @cite </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Raimondi2013acid</t>
-    </r>
-  </si>
-  <si>
     <t>Increase @cite Mountain1990acid @cite Raimondi2013acid</t>
   </si>
   <si>
@@ -884,6 +831,30 @@
   </si>
   <si>
     <t>&lt;/span&gt;|</t>
+  </si>
+  <si>
+    <t>Begin Asthma Attack (Severity 0.7)</t>
+  </si>
+  <si>
+    <t>Administer Albuterol (Albuterol inhaler used correctly, 90.0 ug dose, nozzle loss fraction 0.04)</t>
+  </si>
+  <si>
+    <t>Drug Onset in &lt; 5 min</t>
+  </si>
+  <si>
+    <t>Decrease; @cite bergeronSME Decrease is expected with increased heart rate</t>
+  </si>
+  <si>
+    <t>Increase @cite adams2012patient @cite Raimondi2013acid</t>
+  </si>
+  <si>
+    <t>Decrease @cite adams2012patient @cite Raimondi2013acid</t>
+  </si>
+  <si>
+    <t>Increase back to baseline @cite adams2012patient</t>
+  </si>
+  <si>
+    <t>Back to baseline @cite Mountain1990acid @cite Raimondi2013acid</t>
   </si>
 </sst>
 </file>
@@ -1516,12 +1487,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1540,6 +1505,33 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1552,44 +1544,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1949,20 +1920,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="113"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="108"/>
     </row>
     <row r="2" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="109" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="110"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="105"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1993,52 +1964,52 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="116"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="111"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="110"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="105"/>
     </row>
     <row r="7" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="109"/>
-      <c r="D7" s="110"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="105"/>
     </row>
     <row r="8" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="104" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="109"/>
-      <c r="D8" s="110"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="105"/>
     </row>
     <row r="9" spans="1:4" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="110"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="105"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
@@ -2058,61 +2029,61 @@
       <c r="A12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="112" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="113"/>
     </row>
     <row r="13" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="109"/>
-      <c r="D13" s="110"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="105"/>
     </row>
     <row r="14" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="109"/>
-      <c r="D14" s="110"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="105"/>
     </row>
     <row r="15" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="109"/>
-      <c r="D15" s="110"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="105"/>
     </row>
     <row r="16" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="109" t="s">
+      <c r="B16" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="110"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="105"/>
     </row>
     <row r="17" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="109"/>
-      <c r="D17" s="110"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="105"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
@@ -2126,21 +2097,21 @@
       <c r="A19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="105" t="s">
+      <c r="B19" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="106"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="113"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="107"/>
-      <c r="D20" s="108"/>
+      <c r="C20" s="114"/>
+      <c r="D20" s="115"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
@@ -2186,12 +2157,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B9:D9"/>
@@ -2201,6 +2166,12 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3090,34 +3061,34 @@
       <c r="BM6" s="90"/>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="116" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="117"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
     </row>
     <row r="8" spans="1:65" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="60"/>
       <c r="B8" s="60"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
-      <c r="G8" s="118" t="s">
+      <c r="G8" s="117" t="s">
         <v>161</v>
       </c>
-      <c r="H8" s="118"/>
-      <c r="I8" s="118"/>
-      <c r="J8" s="118"/>
-      <c r="K8" s="118"/>
-      <c r="L8" s="118"/>
-      <c r="M8" s="118"/>
-      <c r="N8" s="118"/>
-      <c r="O8" s="118"/>
-      <c r="P8" s="118"/>
-      <c r="Q8" s="118"/>
-      <c r="R8" s="118"/>
-      <c r="S8" s="118"/>
-      <c r="T8" s="118"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="117"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="117"/>
+      <c r="L8" s="117"/>
+      <c r="M8" s="117"/>
+      <c r="N8" s="117"/>
+      <c r="O8" s="117"/>
+      <c r="P8" s="117"/>
+      <c r="Q8" s="117"/>
+      <c r="R8" s="117"/>
+      <c r="S8" s="117"/>
+      <c r="T8" s="117"/>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="C9" s="62"/>
@@ -3160,433 +3131,434 @@
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AE1" sqref="A1:AE4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18" customWidth="1"/>
-    <col min="27" max="27" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.5703125" customWidth="1"/>
-    <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="118" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="118" customWidth="1"/>
+    <col min="3" max="3" width="2" style="118" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="118" customWidth="1"/>
+    <col min="5" max="5" width="2" style="118" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="118" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="118" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="118" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="118" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="118" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="118" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="118" customWidth="1"/>
+    <col min="13" max="13" width="30.85546875" style="118" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" style="118" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" style="118" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" style="118" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" style="118" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" style="118" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7109375" style="118" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="118" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.7109375" style="118" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" style="118" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.7109375" style="118" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" style="118" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.85546875" style="118" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" style="118" customWidth="1"/>
+    <col min="27" max="27" width="29.7109375" style="118" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18" style="118" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.85546875" style="118" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" style="118" customWidth="1"/>
+    <col min="31" max="31" width="9" style="118" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="118"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="99" t="s">
         <v>167</v>
       </c>
       <c r="B1" s="98" t="s">
         <v>168</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="99" t="s">
         <v>167</v>
       </c>
       <c r="D1" s="98" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" s="99" t="s">
+      <c r="E1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="H1" s="99" t="s">
+      <c r="G1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" s="99" t="s">
+      <c r="I1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="97" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="L1" s="100" t="s">
+      <c r="K1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="L1" s="98" t="s">
+        <v>178</v>
+      </c>
+      <c r="M1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" s="98" t="s">
+        <v>179</v>
+      </c>
+      <c r="O1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="R1" s="98" t="s">
+        <v>180</v>
+      </c>
+      <c r="S1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="T1" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="M1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="N1" s="100" t="s">
+      <c r="U1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="V1" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="O1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="P1" s="100" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="R1" s="100" t="s">
+      <c r="W1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="X1" s="98" t="s">
         <v>183</v>
       </c>
-      <c r="S1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="T1" s="100" t="s">
+      <c r="Y1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z1" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="U1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="V1" s="100" t="s">
+      <c r="AA1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" s="98" t="s">
         <v>185</v>
       </c>
-      <c r="W1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="X1" s="100" t="s">
+      <c r="AC1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD1" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="Y1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z1" s="100" t="s">
+      <c r="AE1" s="99" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="I2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="J2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="M2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="O2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="R2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="S2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="T2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="U2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="V2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="W2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="X2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="AC2" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD2" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE2" s="99" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="99">
+        <v>60</v>
+      </c>
+      <c r="G3" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="99">
+        <v>660</v>
+      </c>
+      <c r="I3" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="J3" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="AA1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="AB1" s="100" t="s">
+      <c r="K3" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" s="102" t="s">
+        <v>205</v>
+      </c>
+      <c r="M3" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="N3" s="102" t="s">
+        <v>187</v>
+      </c>
+      <c r="O3" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" s="101" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q3" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="R3" s="101" t="s">
+        <v>193</v>
+      </c>
+      <c r="S3" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="T3" s="102" t="s">
+        <v>206</v>
+      </c>
+      <c r="U3" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="V3" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="AC1" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="AD1" s="100" t="s">
+      <c r="W3" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="X3" s="102" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y3" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z3" s="102" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA3" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB3" s="102" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC3" s="99" t="s">
         <v>189</v>
       </c>
-      <c r="AE1" s="97" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="G2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="H2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="I2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="J2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="L2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="M2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="N2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="O2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="P2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="R2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="S2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="T2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="U2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="V2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="W2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="X2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="AB2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC2" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="AD2" s="100" t="s">
-        <v>174</v>
-      </c>
-      <c r="AE2" s="97" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" s="101">
-        <v>60</v>
-      </c>
-      <c r="G3" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="H3" s="101">
+      <c r="AD3" s="100" t="s">
+        <v>199</v>
+      </c>
+      <c r="AE3" s="99" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="78" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="99">
         <v>660</v>
       </c>
-      <c r="I3" s="97" t="s">
-        <v>175</v>
-      </c>
-      <c r="J3" s="104" t="s">
+      <c r="G4" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="99">
+        <v>960</v>
+      </c>
+      <c r="I4" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="J4" s="100" t="s">
+        <v>188</v>
+      </c>
+      <c r="K4" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="101" t="s">
+        <v>192</v>
+      </c>
+      <c r="M4" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="N4" s="101" t="s">
+        <v>188</v>
+      </c>
+      <c r="O4" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="L3" s="104" t="s">
-        <v>195</v>
-      </c>
-      <c r="M3" s="97" t="s">
+      <c r="P4" s="102" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q4" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="R4" s="101" t="s">
+        <v>192</v>
+      </c>
+      <c r="S4" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="N3" s="104" t="s">
-        <v>190</v>
-      </c>
-      <c r="O3" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="P3" s="103" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q3" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="R3" s="103" t="s">
+      <c r="T4" s="102" t="s">
+        <v>207</v>
+      </c>
+      <c r="U4" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="V4" s="102" t="s">
+        <v>208</v>
+      </c>
+      <c r="W4" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="X4" s="101" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y4" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z4" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA4" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB4" s="102" t="s">
         <v>197</v>
       </c>
-      <c r="S3" s="97" t="s">
+      <c r="AC4" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="T3" s="104" t="s">
-        <v>200</v>
-      </c>
-      <c r="U3" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="V3" s="104" t="s">
-        <v>198</v>
-      </c>
-      <c r="W3" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="X3" s="104" t="s">
-        <v>202</v>
-      </c>
-      <c r="Y3" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z3" s="104" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA3" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="AB3" s="104" t="s">
-        <v>206</v>
-      </c>
-      <c r="AC3" s="97" t="s">
-        <v>192</v>
-      </c>
-      <c r="AD3" s="102" t="s">
-        <v>208</v>
-      </c>
-      <c r="AE3" s="97" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="78" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="78" t="s">
-        <v>180</v>
-      </c>
-      <c r="E4" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="F4" s="101">
-        <v>660</v>
-      </c>
-      <c r="G4" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="H4" s="101">
-        <v>960</v>
-      </c>
-      <c r="I4" s="97" t="s">
-        <v>193</v>
-      </c>
-      <c r="J4" s="102" t="s">
-        <v>191</v>
-      </c>
-      <c r="K4" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="L4" s="103" t="s">
-        <v>196</v>
-      </c>
-      <c r="M4" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="N4" s="103" t="s">
-        <v>191</v>
-      </c>
-      <c r="O4" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="P4" s="104" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q4" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="R4" s="103" t="s">
-        <v>196</v>
-      </c>
-      <c r="S4" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="T4" s="104" t="s">
+      <c r="AD4" s="102" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE4" s="119" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="V4" s="104" t="s">
-        <v>199</v>
-      </c>
-      <c r="W4" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="X4" s="103" t="s">
-        <v>209</v>
-      </c>
-      <c r="Y4" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z4" s="104" t="s">
-        <v>204</v>
-      </c>
-      <c r="AA4" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="AB4" s="104" t="s">
-        <v>205</v>
-      </c>
-      <c r="AC4" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD4" s="104" t="s">
-        <v>207</v>
-      </c>
-      <c r="AE4" s="120" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AD5" s="119"/>
-      <c r="AE5" s="121"/>
+      <c r="AD5" s="103"/>
+      <c r="AE5" s="120"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AE6" s="121"/>
+      <c r="AE6" s="120"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AE7" s="15"/>
+      <c r="AE7" s="121"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
One more fix to showcase and system methodology.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\Showcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E80D08-D6F6-420A-BB7D-C5A8E2AD1815}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C0C6E7-910F-4964-8062-BB39FECD2C1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="24825" windowHeight="11385" tabRatio="406" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="208">
   <si>
     <t>Scenario Overview</t>
   </si>
@@ -752,9 +752,6 @@
     <t>---</t>
   </si>
   <si>
-    <t>|&lt;span class="success"&gt;</t>
-  </si>
-  <si>
     <t>&lt;/span&gt;|&lt;span class="success"&gt;</t>
   </si>
   <si>
@@ -795,9 +792,6 @@
   </si>
   <si>
     <t>&lt;/span&gt;|&lt;span class="danger"&gt;</t>
-  </si>
-  <si>
-    <t>|&lt;span class="danger"&gt;</t>
   </si>
   <si>
     <t>&lt;/span&gt;|&lt;span class="warning"&gt;</t>
@@ -1223,7 +1217,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1561,6 +1555,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3130,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820C7F09-B001-4E49-B466-E1E2EF602302}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection sqref="A1:AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,13 +3202,13 @@
         <v>167</v>
       </c>
       <c r="L1" s="98" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" s="98" t="s">
         <v>178</v>
-      </c>
-      <c r="M1" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="N1" s="98" t="s">
-        <v>179</v>
       </c>
       <c r="O1" s="99" t="s">
         <v>167</v>
@@ -3223,43 +3220,43 @@
         <v>167</v>
       </c>
       <c r="R1" s="98" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="T1" s="98" t="s">
         <v>180</v>
       </c>
-      <c r="S1" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="T1" s="98" t="s">
+      <c r="U1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="V1" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="U1" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="V1" s="98" t="s">
+      <c r="W1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="X1" s="98" t="s">
         <v>182</v>
       </c>
-      <c r="W1" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="X1" s="98" t="s">
+      <c r="Y1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z1" s="98" t="s">
         <v>183</v>
       </c>
-      <c r="Y1" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z1" s="98" t="s">
+      <c r="AA1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB1" s="98" t="s">
         <v>184</v>
       </c>
-      <c r="AA1" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="AB1" s="98" t="s">
+      <c r="AC1" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD1" s="98" t="s">
         <v>185</v>
-      </c>
-      <c r="AC1" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="AD1" s="98" t="s">
-        <v>186</v>
       </c>
       <c r="AE1" s="99" t="s">
         <v>167</v>
@@ -3365,13 +3362,13 @@
         <v>167</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C3" s="99" t="s">
         <v>167</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="99" t="s">
         <v>167</v>
@@ -3385,74 +3382,74 @@
       <c r="H3" s="99">
         <v>660</v>
       </c>
-      <c r="I3" s="99" t="s">
+      <c r="I3" s="122" t="s">
         <v>175</v>
       </c>
       <c r="J3" s="102" t="s">
+        <v>186</v>
+      </c>
+      <c r="K3" s="122" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" s="102" t="s">
+        <v>203</v>
+      </c>
+      <c r="M3" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="N3" s="102" t="s">
+        <v>186</v>
+      </c>
+      <c r="O3" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="P3" s="101" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q3" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="R3" s="101" t="s">
+        <v>191</v>
+      </c>
+      <c r="S3" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="T3" s="102" t="s">
+        <v>204</v>
+      </c>
+      <c r="U3" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="V3" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="L3" s="102" t="s">
-        <v>205</v>
-      </c>
-      <c r="M3" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="N3" s="102" t="s">
-        <v>187</v>
-      </c>
-      <c r="O3" s="99" t="s">
-        <v>191</v>
-      </c>
-      <c r="P3" s="101" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q3" s="99" t="s">
-        <v>191</v>
-      </c>
-      <c r="R3" s="101" t="s">
+      <c r="W3" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="X3" s="102" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y3" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z3" s="102" t="s">
         <v>193</v>
       </c>
-      <c r="S3" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="T3" s="102" t="s">
-        <v>206</v>
-      </c>
-      <c r="U3" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="V3" s="102" t="s">
+      <c r="AA3" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB3" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC3" s="99" t="s">
         <v>188</v>
       </c>
-      <c r="W3" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="X3" s="102" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y3" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z3" s="102" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA3" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="AB3" s="102" t="s">
-        <v>198</v>
-      </c>
-      <c r="AC3" s="99" t="s">
-        <v>189</v>
-      </c>
       <c r="AD3" s="100" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE3" s="99" t="s">
         <v>199</v>
-      </c>
-      <c r="AE3" s="99" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="75" x14ac:dyDescent="0.25">
@@ -3460,13 +3457,13 @@
         <v>167</v>
       </c>
       <c r="B4" s="78" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C4" s="99" t="s">
         <v>167</v>
       </c>
       <c r="D4" s="78" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E4" s="99" t="s">
         <v>167</v>
@@ -3480,74 +3477,74 @@
       <c r="H4" s="99">
         <v>960</v>
       </c>
-      <c r="I4" s="99" t="s">
+      <c r="I4" s="122" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="K4" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="L4" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="J4" s="100" t="s">
-        <v>188</v>
-      </c>
-      <c r="K4" s="99" t="s">
-        <v>191</v>
-      </c>
-      <c r="L4" s="101" t="s">
-        <v>192</v>
-      </c>
       <c r="M4" s="99" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N4" s="101" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O4" s="99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P4" s="102" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q4" s="99" t="s">
-        <v>191</v>
+        <v>187</v>
+      </c>
+      <c r="Q4" s="122" t="s">
+        <v>175</v>
       </c>
       <c r="R4" s="101" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="S4" s="99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T4" s="102" t="s">
+        <v>205</v>
+      </c>
+      <c r="U4" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="V4" s="102" t="s">
+        <v>206</v>
+      </c>
+      <c r="W4" s="99" t="s">
+        <v>189</v>
+      </c>
+      <c r="X4" s="101" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y4" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="Z4" s="102" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA4" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB4" s="102" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC4" s="99" t="s">
+        <v>175</v>
+      </c>
+      <c r="AD4" s="102" t="s">
         <v>207</v>
       </c>
-      <c r="U4" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="V4" s="102" t="s">
-        <v>208</v>
-      </c>
-      <c r="W4" s="99" t="s">
-        <v>191</v>
-      </c>
-      <c r="X4" s="101" t="s">
-        <v>200</v>
-      </c>
-      <c r="Y4" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z4" s="102" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA4" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="AB4" s="102" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC4" s="99" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD4" s="102" t="s">
-        <v>209</v>
-      </c>
       <c r="AE4" s="119" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final update to the matrices and system methdodology.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/Showcases/AsthmaAttackValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\Showcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C0C6E7-910F-4964-8062-BB39FECD2C1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CDA36C-6615-4083-94DF-C96010FF9081}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="24825" windowHeight="11385" tabRatio="406" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -806,18 +806,6 @@
     <t>Decreased peak @cite Nowak1983arterial</t>
   </si>
   <si>
-    <t>71.5 ± 12 @cite Nowak1983arterial</t>
-  </si>
-  <si>
-    <t>78.0 ± 12.7 @cite Nowak1983arterial</t>
-  </si>
-  <si>
-    <t>32.3 ± 4.6 @cite Nowak1983arterial</t>
-  </si>
-  <si>
-    <t>35.8 ± 6.9 @cite Nowak1983arterial</t>
-  </si>
-  <si>
     <t>Increase @cite Mountain1990acid @cite Raimondi2013acid</t>
   </si>
   <si>
@@ -849,6 +837,18 @@
   </si>
   <si>
     <t>Back to baseline @cite Mountain1990acid @cite Raimondi2013acid</t>
+  </si>
+  <si>
+    <t>71.5&amp;plusmn; 12 @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <t>78.0 &amp;plusmn; 12.7 @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <t>35.8 &amp;plusmn;6.9 @cite Nowak1983arterial</t>
+  </si>
+  <si>
+    <t>32.3 &amp;plusmn; 4.6 @cite Nowak1983arterial</t>
   </si>
 </sst>
 </file>
@@ -3362,7 +3362,7 @@
         <v>167</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C3" s="99" t="s">
         <v>167</v>
@@ -3392,7 +3392,7 @@
         <v>175</v>
       </c>
       <c r="L3" s="102" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="M3" s="99" t="s">
         <v>175</v>
@@ -3416,7 +3416,7 @@
         <v>175</v>
       </c>
       <c r="T3" s="102" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="U3" s="99" t="s">
         <v>175</v>
@@ -3434,22 +3434,22 @@
         <v>175</v>
       </c>
       <c r="Z3" s="102" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="AA3" s="99" t="s">
         <v>175</v>
       </c>
       <c r="AB3" s="102" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="AC3" s="99" t="s">
         <v>188</v>
       </c>
       <c r="AD3" s="100" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="AE3" s="99" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="75" x14ac:dyDescent="0.25">
@@ -3457,13 +3457,13 @@
         <v>167</v>
       </c>
       <c r="B4" s="78" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C4" s="99" t="s">
         <v>167</v>
       </c>
       <c r="D4" s="78" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E4" s="99" t="s">
         <v>167</v>
@@ -3511,40 +3511,40 @@
         <v>175</v>
       </c>
       <c r="T4" s="102" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="U4" s="99" t="s">
         <v>175</v>
       </c>
       <c r="V4" s="102" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="W4" s="99" t="s">
         <v>189</v>
       </c>
       <c r="X4" s="101" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="Y4" s="99" t="s">
         <v>175</v>
       </c>
       <c r="Z4" s="102" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="AA4" s="99" t="s">
         <v>175</v>
       </c>
       <c r="AB4" s="102" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="AC4" s="99" t="s">
         <v>175</v>
       </c>
       <c r="AD4" s="102" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AE4" s="119" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>